<commit_message>
atuando nos dois primeiros passos da segunda fase
</commit_message>
<xml_diff>
--- a/docs/CRESCER/Relatório.xlsx
+++ b/docs/CRESCER/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,83 +504,202 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+          <t>Folha analítica -&gt; Planilha</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CLAYDERMAN DE OLIVEIRA FELISBERTO</t>
+          <t>Nome</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Profissional não encontrado pelo CPF</t>
+          <t>Profissional na folha analítica e fora da planilha</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+          <t>Folha analítica -&gt; Planilha</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ENEIDA SANTOS DE OLIVEIRA</t>
+          <t>Salário Liquido</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Profissional não encontrado pelo CPF</t>
+          <t>Profissional na folha analítica e fora da planilha</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+          <t>Folha analítica -&gt; Planilha</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>JHONATAN MESQUITA DE ARAUJO</t>
+          <t>Cargo</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Profissional não encontrado pelo CPF</t>
+          <t>Profissional na folha analítica e fora da planilha</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+          <t>Folha analítica -&gt; Planilha</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>JULIANA MICHELLE ANIBAL ALVES</t>
+          <t>Data_Admissão</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Profissional não encontrado pelo CPF</t>
+          <t>Profissional na folha analítica e fora da planilha</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Folha analítica -&gt; Planilha</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Matrícula</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Profissional na folha analítica e fora da planilha</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CLAYDERMAN DE OLIVEIRA FELISBERTO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Erro no CPF ou matrícula</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ENEIDA SANTOS DE OLIVEIRA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Erro no CPF ou matrícula</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>JHONATAN MESQUITA DE ARAUJO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Erro no CPF ou matrícula</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Folha analítica -&gt; Comprovante de pagamento</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JULIANA MICHELLE ANIBAL ALVES</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Erro no CPF ou matrícula</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Comprovante de pagamento -&gt; Folha analítica</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NOME CPF</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Profissional na folha analítica e fora da planilha</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Comprovante de pagamento -&gt; Folha analítica</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>VALOR</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Profissional na folha analítica e fora da planilha</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>Planilha -&gt; GFIP - SEFIP</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>HAROLDO GONCALVES DA SILVA</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Profissional não encontrado pelo PIS/PASEP</t>
         </is>

</xml_diff>